<commit_message>
revise get value from data table
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestingTestData.xlsx
+++ b/Assets/Excel/SmokeTestingTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD396EC6-C436-4BE0-89A0-272548CFC167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B80EC0-7850-48D8-8F27-647866387800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Credential" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>First Name</t>
   </si>
@@ -50,15 +50,6 @@
     <t>MRN</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Cellphone Number</t>
-  </si>
-  <si>
-    <t>Email Address</t>
-  </si>
-  <si>
     <t>Middle Name</t>
   </si>
   <si>
@@ -156,6 +147,24 @@
   </si>
   <si>
     <t>Barcode</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>CellphoneNumber</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
   </si>
 </sst>
 </file>
@@ -546,25 +555,25 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -576,54 +585,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92BB898-03AF-4314-BBE1-C81D9493E022}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>1111111111</v>
@@ -632,15 +641,15 @@
         <v>2222222222</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -655,59 +664,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC41914-52A6-4FDD-A918-4FCC1614BE99}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="2"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="3">
         <v>35848</v>
@@ -722,7 +731,7 @@
         <v>100</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I2">
         <v>123</v>
@@ -731,12 +740,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>1234</v>
@@ -748,7 +757,7 @@
         <v>200</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>123</v>
@@ -767,51 +776,51 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C2" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add guardian tab additional column
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestingTestData.xlsx
+++ b/Assets/Excel/SmokeTestingTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB7620C-46AD-4FAA-A984-26120E866E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93091FD-4648-4114-BB0F-5D568CE25768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Credential" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>MRN</t>
   </si>
@@ -546,12 +546,12 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -559,7 +559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -574,22 +574,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92BB898-03AF-4314-BBE1-C81D9493E022}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -611,8 +612,11 @@
       <c r="G1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -634,8 +638,11 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="3">
+        <v>27051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -655,19 +662,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC41914-52A6-4FDD-A918-4FCC1614BE99}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="2"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -702,7 +709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -731,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -767,17 +774,17 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -797,7 +804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Update type date of birth logic
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestingTestData.xlsx
+++ b/Assets/Excel/SmokeTestingTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93091FD-4648-4114-BB0F-5D568CE25768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D627A81-E7E1-49CB-BB77-E246BD799573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Credential" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>MRN</t>
   </si>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92BB898-03AF-4314-BBE1-C81D9493E022}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC41914-52A6-4FDD-A918-4FCC1614BE99}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3">
-        <v>35848</v>
+        <v>45344</v>
       </c>
       <c r="E2">
         <v>123</v>
@@ -731,8 +731,8 @@
       <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2">
-        <v>123</v>
+      <c r="I2" t="s">
+        <v>25</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -757,8 +757,8 @@
       <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I3">
-        <v>123</v>
+      <c r="I3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Water + Fortifier + Modular
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestingTestData.xlsx
+++ b/Assets/Excel/SmokeTestingTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Documents\UiPath\TMNP Smoke Testing Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F2793E-9D8F-4294-BCFC-ACF117F66FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E038D23-DE4B-4F7C-9707-B00A6AA3BA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1710" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Credential" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="673">
   <si>
     <t>MRN</t>
   </si>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3130,13 +3130,16 @@
       <c r="C21" t="s">
         <v>670</v>
       </c>
-      <c r="E21" t="e">
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="str">
         <f>IF(VLOOKUP(D21, 'Order Base'!A:B, 2, FALSE)=0, "", VLOOKUP(D21, 'Order Base'!A:B, 2, FALSE))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F21" t="e">
+        <v>Sim Sterile Water</v>
+      </c>
+      <c r="F21">
         <f>VLOOKUP(D21, 'Order Base'!A:C, 3, FALSE)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="G21" s="4">
         <v>10</v>
@@ -3207,7 +3210,7 @@
           <x14:formula1>
             <xm:f>'Order Base'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:D12 D15</xm:sqref>
+          <xm:sqref>D11:D12 D15 D21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
API-5614: Fix unable to prepare issue
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestingTestData.xlsx
+++ b/Assets/Excel/SmokeTestingTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation for peer review\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A8987B-8914-4343-B313-4A66DD68DC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F65E97-27A7-452A-9B42-24DE6097C680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Guardian" sheetId="1" r:id="rId1"/>
@@ -2505,7 +2505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92BB898-03AF-4314-BBE1-C81D9493E022}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -2731,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31380DA0-60E8-49BA-9807-75EAC6F400B7}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2890,7 +2890,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="7">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2995,7 +2995,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="7">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -3101,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="7">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -3257,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="L26" s="7">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -3385,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="L32" s="7">
-        <v>5</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AUTOMATE-32: Added cal conversion to fix error on add order
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestingTestData.xlsx
+++ b/Assets/Excel/SmokeTestingTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28E255E-28FA-449F-ACA1-F07D92735470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2177270-5AA9-4B80-9B5E-7842AAF9BC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
+    <workbookView xWindow="-51720" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{DAEDCE94-5880-43BD-9814-69B501689CEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Guardian" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Order" sheetId="4" r:id="rId3"/>
     <sheet name="Order Base" sheetId="5" r:id="rId4"/>
     <sheet name="OrderAdditives" sheetId="6" r:id="rId5"/>
+    <sheet name="Setup" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="681">
   <si>
     <t>MRN</t>
   </si>
@@ -2062,13 +2063,34 @@
   </si>
   <si>
     <t>MPID</t>
+  </si>
+  <si>
+    <t>Settings Name</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>cal_per_oz_unit_conversion</t>
+  </si>
+  <si>
+    <t>KCAL_PER_100_MLS</t>
+  </si>
+  <si>
+    <t>KCAL_PER_OZ_DEFAULT</t>
+  </si>
+  <si>
+    <t>KCAL_PER_ML</t>
+  </si>
+  <si>
+    <t>ui/decimal/rounding/cals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2091,6 +2113,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1F2226"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2120,7 +2149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2145,6 +2174,13 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2512,7 +2548,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,7 +2808,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,6 +2896,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -2878,6 +2915,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 24*Setup!F2, IF(Setup!B2=Setup!E1, 24*Setup!E2, IF(Setup!B2=Setup!D1, 24*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>24</v>
       </c>
     </row>
@@ -2912,6 +2950,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -2965,6 +3004,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -2983,6 +3023,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 24*Setup!F2, IF(Setup!B2=Setup!E1, 24*Setup!E2, IF(Setup!B2=Setup!D1, 24*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>24</v>
       </c>
     </row>
@@ -3017,6 +3058,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -3070,6 +3112,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -3088,6 +3131,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 24*Setup!F2, IF(Setup!B2=Setup!E1, 24*Setup!E2, IF(Setup!B2=Setup!D1, 24*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>24</v>
       </c>
     </row>
@@ -3123,6 +3167,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -3213,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="7">
-        <f>E20+2</f>
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -3232,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="L23" s="7">
-        <f>E21+4</f>
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 24*Setup!F2, IF(Setup!B2=Setup!E1, 24*Setup!E2, IF(Setup!B2=Setup!D1, 24*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>24</v>
       </c>
     </row>
@@ -3278,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="7">
-        <f>E24+2</f>
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -3344,6 +3389,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 20*Setup!F2, IF(Setup!B2=Setup!E1, 20*Setup!E2, IF(Setup!B2=Setup!D1, 20*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>20</v>
       </c>
     </row>
@@ -3362,6 +3408,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 22*Setup!F2, IF(Setup!B2=Setup!E1, 22*Setup!E2, IF(Setup!B2=Setup!D1, 22*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>22</v>
       </c>
     </row>
@@ -3407,6 +3454,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="7">
+        <f>IFERROR(ROUND(IF(Setup!B2=Setup!F1, 20*Setup!F2, IF(Setup!B2=Setup!E1, 20*Setup!E2, IF(Setup!B2=Setup!D1, 20*Setup!D2, 0))), IF(Setup!B2=Setup!D1, 0, Setup!B3)), 0)</f>
         <v>20</v>
       </c>
     </row>
@@ -8490,4 +8538,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588C229F-E3EA-442A-809A-364CBB32564D}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="12" t="s">
+        <v>678</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>676</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <f>1 / 29.5735296</f>
+        <v>3.3814022658965943E-2</v>
+      </c>
+      <c r="F2" s="11">
+        <f>1 / (29.5735296 / 100)</f>
+        <v>3.3814022658965945</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{C5A0D655-FFA3-4DC8-9CA5-A4380E37F444}">
+      <formula1>$D$1:$F$1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>